<commit_message>
Add files for version 1.0.
</commit_message>
<xml_diff>
--- a/06-verification/Problem Report Status.xlsx
+++ b/06-verification/Problem Report Status.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kander4\Documents\MIDI-Router\05-verification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kand4\Dropbox\electronics\in-process\MIDI-Router\06-verification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F362C3-BA47-4C31-ADA0-B3FC69AD4C00}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF2172F-0BE7-4EBD-BECB-A09527AD0123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01F44502-D890-40F0-99CD-8DF1ED07B517}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>Problem Report</t>
   </si>
@@ -103,6 +103,84 @@
   </si>
   <si>
     <t>PCB - I2C</t>
+  </si>
+  <si>
+    <t>PR-006</t>
+  </si>
+  <si>
+    <t>Missing MIDI</t>
+  </si>
+  <si>
+    <t>No MIDI output observed in behavior of synthesizer.</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>PR-007</t>
+  </si>
+  <si>
+    <t>Missing MIDI Data</t>
+  </si>
+  <si>
+    <t>Missing MIDI note data at the synthesizer.</t>
+  </si>
+  <si>
+    <t>PR-008</t>
+  </si>
+  <si>
+    <t>All functions missing</t>
+  </si>
+  <si>
+    <t>Systems appears to have crashed. Recovered after a power cycle.</t>
+  </si>
+  <si>
+    <t>PR-009</t>
+  </si>
+  <si>
+    <t>SS not aligned to SCK</t>
+  </si>
+  <si>
+    <t>SS provides plenty of time ahead of SCK, but it doesn't deassert when SCK does.</t>
+  </si>
+  <si>
+    <t>PR-010</t>
+  </si>
+  <si>
+    <t>FPGA app</t>
+  </si>
+  <si>
+    <t>LD not functioning</t>
+  </si>
+  <si>
+    <t>LD doesn't function, which prevents reads from occurring.</t>
+  </si>
+  <si>
+    <t>PR-011</t>
+  </si>
+  <si>
+    <t>Error in fourth data exchange</t>
+  </si>
+  <si>
+    <t>Incorrect value exchanged on SPI bus on fourth transaction</t>
+  </si>
+  <si>
+    <t>PR-012</t>
+  </si>
+  <si>
+    <t>Synthesizer doesn't see data</t>
+  </si>
+  <si>
+    <t>Data looks OK on the logic analyzer, but the synthesizer doesn't see the data.</t>
+  </si>
+  <si>
+    <t>PR-013</t>
+  </si>
+  <si>
+    <t>FPGA doesn't drive MIDI out 0</t>
+  </si>
+  <si>
+    <t>FPGA is able to drive output on pin 29, but not on pin 26</t>
   </si>
 </sst>
 </file>
@@ -138,9 +216,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70E0E73-8351-4979-AE3E-866C8A049AC7}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,8 +545,8 @@
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -605,6 +684,190 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44282</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44288</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44288</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44295</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44303</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44303</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44317</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44331</v>
+      </c>
+      <c r="B10" s="2">
+        <v>44349</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44349</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44349</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44349</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44379</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44406</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44429</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>